<commit_message>
Move to new command protocol. ADD: Timelapse setup.
</commit_message>
<xml_diff>
--- a/Costs.xlsx
+++ b/Costs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Кирилл</t>
   </si>
@@ -402,7 +402,7 @@
   <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,9 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>4195.2</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
@@ -433,7 +435,9 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="4">
         <v>1670</v>
       </c>

</xml_diff>